<commit_message>
updated weight loss tracker
</commit_message>
<xml_diff>
--- a/Weight_Loss_Journey.xlsx
+++ b/Weight_Loss_Journey.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Haig\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Haig\OneDrive\Desktop\Misc\VS Code Projects\Weight_Loss_Prediction_Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FA4A27F-2E0D-4899-B697-11A97DC14ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC1C433-E06A-4924-B825-78043C15711B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9AD97C05-9611-4D4A-87BD-EA833F2B5741}"/>
   </bookViews>
@@ -394,9 +394,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36103FFB-0C3D-418E-A2F0-4ACEA71BB9CF}">
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:B82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1052,6 +1054,14 @@
         <v>215</v>
       </c>
     </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
+        <v>45326</v>
+      </c>
+      <c r="B82">
+        <v>214</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>